<commit_message>
MVC UPDATE FIX RABU
</commit_message>
<xml_diff>
--- a/temp_doc/PESERTA UJIAN FIX ADMIN.xlsx
+++ b/temp_doc/PESERTA UJIAN FIX ADMIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/cbt2.0admin/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2534FA5C-2A8F-4E42-9442-CBCE9E29FBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9BD72D-B7E3-6C40-86A8-C6FA7AAB6700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{A7D75AB7-B047-3448-8A7B-4FE35F9227AE}"/>
   </bookViews>
@@ -9422,7 +9422,7 @@
     <t>2039218064</t>
   </si>
   <si>
-    <t>SAS2023TH#</t>
+    <t>SAS2023TH*</t>
   </si>
 </sst>
 </file>
@@ -9806,7 +9806,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G1040"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
MV UPDATE FIX KAMIS
</commit_message>
<xml_diff>
--- a/temp_doc/PESERTA UJIAN FIX ADMIN.xlsx
+++ b/temp_doc/PESERTA UJIAN FIX ADMIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/cbt2.0admin/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9BD72D-B7E3-6C40-86A8-C6FA7AAB6700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6422810-3386-B644-930F-C89A120676BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{A7D75AB7-B047-3448-8A7B-4FE35F9227AE}"/>
   </bookViews>
@@ -9422,7 +9422,7 @@
     <t>2039218064</t>
   </si>
   <si>
-    <t>SAS2023TH*</t>
+    <t>SAS2023TH</t>
   </si>
 </sst>
 </file>
@@ -9806,7 +9806,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G1040"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>